<commit_message>
Have written testscript for Product transaction report both in original script and also in ProductTransactionReport Class
</commit_message>
<xml_diff>
--- a/target/test-classes/testdata.xlsx
+++ b/target/test-classes/testdata.xlsx
@@ -9,7 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="DashboardData" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="CategoryData" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t xml:space="preserve">email</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t xml:space="preserve">gmail@2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category Name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category Image</t>
   </si>
 </sst>
 </file>
@@ -172,16 +178,16 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="46.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="0.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="47.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="0.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -255,17 +261,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="C2:C5 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="1.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="0.64"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>